<commit_message>
Dernier commit le lendemain de la compétition avec Shiny app
</commit_message>
<xml_diff>
--- a/matrice_f1.xlsx
+++ b/matrice_f1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielcrepeaut-cauchon/Box Sync/ML-Meet_up/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F585738-992C-8D4F-8AAF-F11BC5AC9CC6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9C25C-3BCB-9D4C-9C60-80963468B966}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{9A3BD3F0-914A-FE43-B629-C43695D4FB54}"/>
   </bookViews>
@@ -25,16 +25,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>Treshold</t>
+  </si>
+  <si>
+    <t>seuil d'importance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,8 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,332 +388,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEEE7E89-F7BB-4C4E-A75F-3241F277FCFE}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="C6:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E7">
         <v>0.15</v>
       </c>
-      <c r="C1">
+      <c r="F7">
         <v>0.2</v>
       </c>
-      <c r="D1">
+      <c r="G7">
         <v>0.25</v>
       </c>
-      <c r="E1">
+      <c r="H7">
         <v>0.3</v>
       </c>
-      <c r="F1">
+      <c r="I7">
         <v>0.35</v>
       </c>
-      <c r="G1">
+      <c r="J7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>0.5</v>
       </c>
-      <c r="B2">
+      <c r="E8">
         <v>0.38591120000000001</v>
       </c>
-      <c r="C2">
+      <c r="F8">
         <v>0.35497840000000003</v>
       </c>
-      <c r="D2">
+      <c r="G8">
         <v>0.17307690000000001</v>
       </c>
-      <c r="E2">
+      <c r="H8">
         <v>4.1666670000000003E-2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
+      <c r="D9">
         <v>0.6</v>
       </c>
-      <c r="B3">
+      <c r="E9">
         <v>0.3846154</v>
       </c>
-      <c r="C3">
+      <c r="F9">
         <v>0.34841630000000001</v>
       </c>
-      <c r="D3">
+      <c r="G9">
         <v>0.24034330000000001</v>
       </c>
-      <c r="E3">
+      <c r="H9">
         <v>2.702703E-2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+      <c r="D10">
         <v>0.7</v>
       </c>
-      <c r="B4">
+      <c r="E10">
         <v>0.37755100000000003</v>
       </c>
-      <c r="C4">
+      <c r="F10">
         <v>0.31797239999999999</v>
       </c>
-      <c r="D4">
+      <c r="G10">
         <v>0.27237349999999999</v>
       </c>
-      <c r="E4">
+      <c r="H10">
         <v>0.11042945</v>
       </c>
-      <c r="F4">
+      <c r="I10">
         <v>1.4705879999999999E-2</v>
       </c>
-      <c r="G4">
+      <c r="J10">
         <v>1.515152E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+      <c r="D11">
         <v>0.8</v>
       </c>
-      <c r="B5">
+      <c r="E11">
         <v>0.38431369999999998</v>
       </c>
-      <c r="C5">
+      <c r="F11">
         <v>0.38071070000000001</v>
       </c>
-      <c r="D5">
+      <c r="G11">
         <v>0.28571429999999998</v>
       </c>
-      <c r="E5">
+      <c r="H11">
         <v>0.26905829999999997</v>
       </c>
-      <c r="F5">
+      <c r="I11">
         <v>0.16279070000000001</v>
       </c>
-      <c r="G5">
+      <c r="J11">
         <v>9.3333330000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+      <c r="D12">
         <v>0.9</v>
       </c>
-      <c r="B6">
+      <c r="E12">
         <v>0.32323229999999997</v>
       </c>
-      <c r="C6">
+      <c r="F12">
         <v>0.31460670000000002</v>
       </c>
-      <c r="D6">
+      <c r="G12">
         <v>0.29102169999999999</v>
       </c>
-      <c r="E6">
+      <c r="H12">
         <v>0.27083332999999998</v>
       </c>
-      <c r="F6">
+      <c r="I12">
         <v>0.2734375</v>
       </c>
-      <c r="G6">
+      <c r="J12">
         <v>0.25641026</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+      <c r="D13">
         <v>0.95</v>
       </c>
-      <c r="B7">
+      <c r="E13">
         <v>0.3148688</v>
       </c>
-      <c r="C7">
+      <c r="F13">
         <v>0.32415899999999997</v>
       </c>
-      <c r="D7">
+      <c r="G13">
         <v>0.30476189999999997</v>
       </c>
-      <c r="E7">
+      <c r="H13">
         <v>0.27906976999999999</v>
       </c>
-      <c r="F7">
+      <c r="I13">
         <v>0.26804124000000001</v>
       </c>
-      <c r="G7">
+      <c r="J13">
         <v>0.26760562999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="B10">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E16">
         <v>0.15</v>
       </c>
-      <c r="C10">
+      <c r="F16">
         <v>0.16</v>
       </c>
-      <c r="D10">
+      <c r="G16">
         <v>0.17</v>
       </c>
-      <c r="E10">
+      <c r="H16">
         <v>0.18</v>
       </c>
-      <c r="F10">
+      <c r="I16">
         <v>0.19</v>
       </c>
-      <c r="G10">
+      <c r="J16">
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
         <v>0.5</v>
       </c>
-      <c r="B11">
+      <c r="E17">
         <v>0.38591120000000001</v>
       </c>
-      <c r="C11">
+      <c r="F17">
         <v>0.38679249999999998</v>
       </c>
-      <c r="D11">
+      <c r="G17">
         <v>0.38048779999999999</v>
       </c>
-      <c r="E11">
+      <c r="H17">
         <v>0.36906850000000002</v>
       </c>
-      <c r="F11">
+      <c r="I17">
         <v>0.35867450000000001</v>
       </c>
-      <c r="G11">
+      <c r="J17">
         <v>0.35497840000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18">
         <v>0.6</v>
       </c>
-      <c r="B12">
+      <c r="E18">
         <v>0.3846154</v>
       </c>
-      <c r="C12">
+      <c r="F18">
         <v>0.3693844</v>
       </c>
-      <c r="D12">
+      <c r="G18">
         <v>0.3738977</v>
       </c>
-      <c r="E12">
+      <c r="H18">
         <v>0.36022510000000002</v>
       </c>
-      <c r="F12">
+      <c r="I18">
         <v>0.35918369999999999</v>
       </c>
-      <c r="G12">
+      <c r="J18">
         <v>0.34841630000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+      <c r="D19">
         <v>0.7</v>
       </c>
-      <c r="B13">
+      <c r="E19">
         <v>0.37755100000000003</v>
       </c>
-      <c r="C13">
+      <c r="F19">
         <v>0.36851519999999999</v>
       </c>
-      <c r="D13">
+      <c r="G19">
         <v>0.37453180000000003</v>
       </c>
-      <c r="E13">
+      <c r="H19">
         <v>0.34412959999999998</v>
       </c>
-      <c r="F13">
+      <c r="I19">
         <v>0.32618029999999998</v>
       </c>
-      <c r="G13">
+      <c r="J19">
         <v>0.31797239999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20">
         <v>0.8</v>
       </c>
-      <c r="B14">
+      <c r="E20">
         <v>0.38431369999999998</v>
       </c>
-      <c r="C14">
+      <c r="F20">
         <v>0.38683129999999999</v>
       </c>
-      <c r="D14">
+      <c r="G20">
         <v>0.38793100000000003</v>
       </c>
-      <c r="E14">
+      <c r="H20">
         <v>0.38443939999999999</v>
       </c>
-      <c r="F14">
+      <c r="I20">
         <v>0.37708829999999999</v>
       </c>
-      <c r="G14">
+      <c r="J20">
         <v>0.38071070000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="D21">
         <v>0.9</v>
       </c>
-      <c r="B15">
+      <c r="E21">
         <v>0.32323229999999997</v>
       </c>
-      <c r="C15">
+      <c r="F21">
         <v>0.3222506</v>
       </c>
-      <c r="D15">
+      <c r="G21">
         <v>0.3157895</v>
       </c>
-      <c r="E15">
+      <c r="H21">
         <v>0.31635390000000002</v>
       </c>
-      <c r="F15">
+      <c r="I21">
         <v>0.31955919999999999</v>
       </c>
-      <c r="G15">
+      <c r="J21">
         <v>0.31460670000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+      <c r="D22">
         <v>0.95</v>
       </c>
-      <c r="B16">
+      <c r="E22">
         <v>0.3148688</v>
       </c>
-      <c r="C16">
+      <c r="F22">
         <v>0.31858409999999998</v>
       </c>
-      <c r="D16">
+      <c r="G22">
         <v>0.32142860000000001</v>
       </c>
-      <c r="E16">
+      <c r="H22">
         <v>0.32432430000000001</v>
       </c>
-      <c r="F16">
+      <c r="I22">
         <v>0.3212121</v>
       </c>
-      <c r="G16">
+      <c r="J22">
         <v>0.32415899999999997</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G7">
+  <mergeCells count="4">
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C17:C22"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E8:J13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -716,7 +770,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:G16">
+  <conditionalFormatting sqref="E17:J22">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>